<commit_message>
Corrections au niveau de la matrice des décisions
</commit_message>
<xml_diff>
--- a/policy_test_apprentissage_corrected.xlsx
+++ b/policy_test_apprentissage_corrected.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Simple :</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>&gt; 21</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
   <si>
     <t>As :</t>
@@ -93,19 +96,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="0"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -136,7 +132,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="008067A2"/>
+        <bgColor rgb="008067A2"/>
       </patternFill>
     </fill>
   </fills>
@@ -164,9 +161,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -182,13 +178,12 @@
     <xf applyAlignment="1" borderId="1" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="41" hidden="0" name="Accent4" xfId="1"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -548,8 +543,8 @@
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="1" t="n">
-        <v>1</v>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1</v>
@@ -1052,7 +1047,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1061,36 +1056,36 @@
     <row r="17" spans="1:16">
       <c r="A17" s="1" t="s"/>
       <c r="B17" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="1" t="n">
-        <v>1</v>
+      <c r="A18" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>1</v>
@@ -1413,7 +1408,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -1422,39 +1417,39 @@
     <row r="31" spans="1:16">
       <c r="A31" s="1" t="s"/>
       <c r="B31" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="1" t="n">
-        <v>1</v>
+      <c r="A32" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>1</v>

</xml_diff>